<commit_message>
Handle decimal numbers in shared strings
</commit_message>
<xml_diff>
--- a/testdata/xlsx_sample.xlsx
+++ b/testdata/xlsx_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -155,7 +155,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -214,8 +214,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,7 +249,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>

</xml_diff>